<commit_message>
Modificação no layout inicial, tutorial, base de dados mesh e alguns bugs
</commit_message>
<xml_diff>
--- a/Data/DADOS_MESH_3D.xlsx
+++ b/Data/DADOS_MESH_3D.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werickson\Desktop\organizar desktop\PROJETOS WERICKSON\Petrobras\Dinam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\PycharmProjects\VDI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8206E464-C683-4757-8E01-5C829C5E9E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D467E7-A294-4166-B57E-382C4F3054D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{13CA9D5F-0C0F-4FD8-AB5B-92513D947E79}"/>
+    <workbookView xWindow="2784" yWindow="228" windowWidth="19944" windowHeight="10956" activeTab="4" xr2:uid="{13CA9D5F-0C0F-4FD8-AB5B-92513D947E79}"/>
   </bookViews>
   <sheets>
-    <sheet name="Siptech 46 cSt" sheetId="1" r:id="rId1"/>
+    <sheet name="Siptech46cSt" sheetId="1" r:id="rId1"/>
     <sheet name="Siptech 35 cSt" sheetId="2" r:id="rId2"/>
     <sheet name="Siptech 90 cSt" sheetId="3" r:id="rId3"/>
     <sheet name="Kerosene 3 cSt" sheetId="4" r:id="rId4"/>
-    <sheet name="Gas oil" sheetId="5" r:id="rId5"/>
+    <sheet name="Gasoil" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -55,7 +55,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +70,27 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -105,34 +126,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +187,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -451,17 +486,17 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,511 +507,511 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1.7350496627624199</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>44.456281613783801</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>44.332436485824097</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1.7666722280451399</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>44.489674129096997</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>45.2517949934876</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1.77930309477624</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>44.5114014499405</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>46.066647016715798</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1.7485834327668801</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>44.5349082618417</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>46.877123739839703</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>1.76570656921</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>44.558230652795999</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>47.641823885761703</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1.84634568451017</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>52.661866665697197</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>46.877648106376803</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1.7866514963624001</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>52.638592521783998</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>46.293497341194502</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1.66172809506853</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>52.632596276026902</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>45.757860008429098</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1.7065152378500399</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>52.657561908486599</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>46.507651744629499</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>1.7726615049647401</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>52.682039561016502</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>47.341616518753298</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1.62182986384524</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>66.256750656010595</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>47.798865203003203</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1.6391986550891</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>66.2287684815619</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>47.240941504668598</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1.6645961346220399</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>66.201490481304702</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>46.706720199433498</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1.57551288389402</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>66.179486344618695</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>46.245453262325697</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>1.5724940488591701</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>66.146406091824602</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>45.560515073330002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1.51213299141069</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>78.378458342095101</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>44.8334865124652</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1.5858478214557501</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>78.385384269421394</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>45.164522437755501</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1.5068068741966201</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>78.1916699832516</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>46.0271419648153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1.57448977452848</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>78.152571208451405</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>46.671368712249901</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>1.421385175545</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>78.222892481469898</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>47.387645548942203</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>1.4514502919310801</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>89.918833164839</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>47.6215406306573</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1.4870508346374001</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>89.909774647457596</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>46.856338874029802</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>1.4770616115973501</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>89.874733574500098</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>45.491974465289999</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>1.4392994116234801</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>89.841727427753298</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>45.001333209709003</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="5">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
         <v>1.4303068194074899</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>89.855476872395997</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>45.481354410323497</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>1.4565895798371</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27">
         <v>101.18014370421599</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>46.613228204821198</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>1.48036064202691</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28">
         <v>101.176587161423</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>47.225032828973198</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1.51492179897069</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>101.06677732562601</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>47.5210903806217</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1.43625516568806</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30">
         <v>101.02407959819099</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>46.8642358098081</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="5">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
         <v>1.42032097286377</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>101.164468293939</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>46.137139982190597</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1.3994228413413501</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32">
         <v>128.78575804322</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>44.830023101027997</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1.43134822934888</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <v>128.763607594028</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>45.175837954814497</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1.40013411808329</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34">
         <v>128.74939749134299</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>45.538847002604498</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>1.4339732716506</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35">
         <v>128.76135663312201</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>45.846016753929803</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="5">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
         <v>1.3628338767166801</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>128.773071354558</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>46.201729545885797</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1.85566098560524</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>37.1137810815246</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>47.522405771393402</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>1.8572174680409199</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>37.091087477058501</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>47.334340033980801</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>1.7917515371691299</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>37.077241314886102</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>46.655435302542699</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>1.8154624711175</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>37.061114539378401</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>46.180545010114898</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>1.80213846051691</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41">
         <v>37.047484724571902</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>45.693432032497199</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -985,21 +1020,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24FBB07-0324-43CA-9971-BDF3AE83AF09}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,409 +1045,409 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1.6673500792806</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>46.376502893731697</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>33.2007059489383</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>1.6315688972259199</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>46.389197234944398</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>33.281514841021298</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>1.6969553578976599</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>46.411547231550998</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>33.700502608935501</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>1.60317395961349</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>46.431553512621001</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>34.045345846141103</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>1.6350481191623101</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>46.448483151288201</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>34.407842434758301</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>1.5917449252524201</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>53.4212142938973</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>34.744196083330799</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>1.5885316889921599</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>53.399850228340398</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>34.475376526185798</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>1.61616847707696</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>53.385159074556398</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>34.199651496467403</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>1.6259453520407801</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>53.385257021095299</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>34.077275998004701</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>1.60789429091537</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>53.395930343995502</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>34.3560272597595</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>1.5018246437581899</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>66.843375086146395</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>34.433454014233199</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>1.52242168380552</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>66.820554093363299</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>34.243349213867603</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>1.5070795740257299</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>66.809115861802994</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>34.035857485719497</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>1.46874314981706</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>66.817945412815206</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>34.204949465823297</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>1.46071220296548</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>66.8437664973697</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>34.511775828976702</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>1.3980778646726599</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>86.187896319482903</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>34.660766979539602</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>1.4185854194743499</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>86.176394337883593</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>34.728360643058402</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>1.4285048961753399</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>86.035906904772105</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>34.745330978553604</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>1.4601423986688999</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>86.121576117146105</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>34.680529244243097</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>1.3997373153095101</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>86.203612069416806</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>34.551593155098999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>1.31744045906324</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>127.79765363148999</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>34.047701570471197</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>1.34024483835616</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>127.8521824564</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>34.042012357052599</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>1.3242482414111101</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>127.82246380110401</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>34.543794743278497</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>1.3320309356993001</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>127.817759761319</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>34.299263643369002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>1.2959446857626</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>127.82296362042599</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>33.783425647021403</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="8"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-      <c r="C34" s="9"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="13"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-      <c r="C40" s="9"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1427,14 +1462,14 @@
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1445,554 +1480,554 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1.9865427042211199</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>77.234017480566806</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>91.191050623103905</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2.0265732605420101</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>77.215330747066901</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>90.770680291026807</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>1.8703558898697501</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>77.200476178265404</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>90.528573576669103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>1.9721048795082301</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>77.175197204360799</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>90.509846837401597</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>1.9085013178636001</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>77.126265409983304</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>90.897875668242406</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>1.9013498857487801</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>87.216510293278404</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>91.328255765777399</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>1.8501752978372701</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>87.211877598422305</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>91.581976566175996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>1.92886670335835</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>87.1831449086704</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>91.915816998892396</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>1.8955661678489999</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>87.176176110124104</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>92.353655289323598</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>1.83322838204662</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>87.170595246591205</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>92.728265776145307</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>1.7771743911525799</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>99.405439014370302</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>93.136157781696596</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>1.7574990801546</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>99.375915158131207</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>92.852759407973494</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>1.7557751494569001</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>99.394472073019898</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>92.249544010258106</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>1.76257140621435</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>99.344406490361607</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>91.919004502288104</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>1.7316855253955099</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>99.359645561481997</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>91.701617411621896</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>1.7340880226069799</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>111.783607881851</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>91.681185135765006</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>1.7104387025265599</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18">
         <v>111.766842509385</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>91.6340455019442</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>1.72192702148469</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>111.781814010169</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>91.632792857485896</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>1.7173931063560299</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>111.812865997033</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>91.638371386826805</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>1.71416429305508</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>111.74234064103599</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>91.6616640007</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>1.65188792229278</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>128.83286145329501</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>91.089681087268104</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>1.48901481461414</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23">
         <v>128.744962097886</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>90.086191928561206</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>1.6639368188913899</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>128.73099947237901</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>89.7311751594535</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>1.6285538391360499</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>128.72153560674701</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>89.382058500725293</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>1.74333018422324</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>128.74388415076999</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6">
         <v>89.914018049813393</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>1.28667444714329</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27">
         <v>47.053689309427398</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>94.806749045136499</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>1.32891547223651</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28">
         <v>47.029066788615602</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>94.431349319337301</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>1.3204769989982601</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>47.0148819251487</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>93.999196596169696</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>1.29080756141092</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30">
         <v>47.001158918214301</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>93.615468106732607</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
         <v>1.2732168983904899</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>47.000354084498703</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>93.359844848677696</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>1.24467732689169</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32">
         <v>28.1408921385414</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>93.137107546731002</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>1.24092087199134</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <v>28.131842023027499</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>92.924110309863806</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>1.18668570501596</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34">
         <v>28.120236571555601</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>92.603921015858305</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>1.2021739169627801</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35">
         <v>28.117158656602101</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>92.337767494776301</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
         <v>1.0560435185710699</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>28.1128373210272</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>92.125663446839496</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>1.99706045783241</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37">
         <v>60.3913419633218</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>91.527019770306296</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>1.9006822707914299</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38">
         <v>60.380322985592599</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>91.325915120219705</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>1.96937348793328</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>60.374990387648403</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>91.142040351851406</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>2.0097870420194202</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40">
         <v>60.374286654106001</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>91.024345270654905</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
         <v>1.9337962616455699</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <v>60.381360317390197</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="6">
         <v>91.166484514999894</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>1.77842831435245</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42">
         <v>53.389259106714803</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>92.089919753441393</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>1.72290294835841</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>53.400538593422901</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>92.6874437720912</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>1.7108967016523899</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44">
         <v>53.414233568401997</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>93.284753460961696</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>1.68620178385898</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>53.424146667693499</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>93.835958847700795</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>1.6672998123165399</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46">
         <v>53.4147593116435</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46">
         <v>93.768313606552994</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2003,18 +2038,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6627F8C-511D-47BC-9621-4E9907C6B28F}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2025,467 +2060,467 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
         <v>1.3544567629178299</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>5.9461090856120098</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>2.6550773816357824</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>1.3916007379853399</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>5.9395203463218396</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>2.6547232631571909</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>1.3976532429240101</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>5.9384557647825602</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>2.6553391737473651</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>1.41874323149105</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>5.93790778356753</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>2.6550503007119368</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>1.38090673551719</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>5.9370321378145503</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>2.6525026426422484</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
         <v>1.42120735872112</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>5.9387539805265197</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>2.6532531379816553</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>1.29603447153512</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>11.282358411836499</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>2.6550851471323083</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>1.3083397981052101</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>11.286540565589</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>2.6546643086563799</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>1.28525936576557</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>11.289985646358</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>2.6558008661297605</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>1.28523455520945</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>11.2899737554136</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>2.6539577352966539</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="8">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>1.3099944369443499</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>11.2910049912088</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <v>2.6499037170536703</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="12">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
         <v>1.2934773768716701</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>11.2914168443465</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>2.6482594044922454</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>1.1915808457291801</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>22.403397383570901</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>2.6506220666778773</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>1.2591924430229999</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>22.419850571334401</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <v>2.6490092705457915</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
         <v>1.22183495773867</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16">
         <v>22.418768003354</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <v>2.6503533064366294</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>1.23579953175234</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17">
         <v>22.4201565144147</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <v>2.6502580367228905</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="12">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
         <v>1.2164283233265201</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>22.4171828188902</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <v>2.6519283904858746</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>1.1788877654941099</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19">
         <v>41.704433555706203</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <v>2.6497293024447668</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="8">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>1.1695061931728901</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20">
         <v>41.7100302931117</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <v>2.6503858754419052</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
         <v>1.2073480133665599</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21">
         <v>41.7100345299271</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>2.6483082326983078</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
         <v>1.1788108564717299</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22">
         <v>41.709132611834598</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>2.6467076088080446</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="12">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
         <v>1.18996685781477</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>41.710490209061199</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>2.6472634333307252</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
         <v>1.1725113336628501</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24">
         <v>77.991721540828394</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <v>2.6359026829682537</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
         <v>1.1638402311795599</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25">
         <v>78.073447609629596</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="13">
         <v>2.6226719290719864</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
         <v>1.2101140226971401</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26">
         <v>77.972644656038</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <v>2.6206465719598251</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
         <v>1.1653452702506599</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27">
         <v>77.875209485622307</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="13">
         <v>2.6201188541941796</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="12">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
         <v>1.12667208682159</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>77.925318612958804</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="13">
         <v>2.6197076056111182</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
         <v>1.10137448507804</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <v>130.95731918746</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="13">
         <v>2.6248219201448815</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="10">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
         <v>1.0691367713900699</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>130.92925625758701</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="13">
         <v>2.6128834819114517</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="10">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9">
         <v>1.1064590620135</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>130.89557826016801</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="13">
         <v>2.6017323361731228</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="8">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
         <v>1.11311286741376</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32">
         <v>130.901220058174</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="13">
         <v>2.5901219413136456</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
         <v>1.0887094677957401</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <v>130.88594333395901</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="13">
         <v>2.5825104076491923</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="8"/>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="8"/>
-      <c r="C35" s="14"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="8"/>
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="C39" s="14"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
-      <c r="C44" s="14"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="8"/>
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
-      <c r="C47" s="14"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="C34" s="13"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="C47" s="13"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2496,423 +2531,423 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E5D556-BD6E-4E58-87B8-5CEC985C4D6C}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>1.23004247445026</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="16">
         <v>129.93745198978101</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="17">
         <v>10.3231296199976</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>1.2102442560017299</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="16">
         <v>129.920234572711</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="17">
         <v>10.3130912052978</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>1.2335948143222999</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="16">
         <v>129.99149016493601</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="17">
         <v>10.355139898122999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>1.22228909371821</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="16">
         <v>130.04702007756401</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="17">
         <v>10.384804398739</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <v>1.2521636205579201</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="16">
         <v>129.991321615576</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="17">
         <v>10.424025509190701</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
         <v>1.24735348451207</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="19">
         <v>130.044349433132</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="20">
         <v>10.4442445079221</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>1.2024100928510799</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="16">
         <v>89.764438018569905</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="17">
         <v>10.6490926293115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
         <v>1.2548694302471199</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="16">
         <v>90.0447842514656</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="17">
         <v>10.7128989138082</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>1.2766953528075999</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="16">
         <v>89.987296840472794</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="17">
         <v>10.6918937192195</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>1.1835657829522901</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="16">
         <v>90.078623313108196</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="17">
         <v>10.667176569317</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
         <v>1.22302192934158</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="19">
         <v>90.088103924624306</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="20">
         <v>10.6479078677123</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="8">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
         <v>1.3391491994038101</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="16">
         <v>65.528867762617296</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="17">
         <v>10.623865711758199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
         <v>1.2837848397462499</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="16">
         <v>65.513566106334594</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="17">
         <v>10.6104169500515</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>1.33592071044466</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="16">
         <v>65.491319906297704</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="17">
         <v>10.5939996737476</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
         <v>1.3166793497244</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="16">
         <v>65.482383963339899</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="17">
         <v>10.577368919054701</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="12">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
         <v>1.25776288997055</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="19">
         <v>65.470993721917097</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="20">
         <v>10.5545075282322</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
         <v>1.37675901727959</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="16">
         <v>39.376652091634</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="17">
         <v>10.5540600322733</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>1.3285275381733901</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="16">
         <v>39.371555119820798</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="17">
         <v>10.5581297666422</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="8">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
         <v>1.3556940216711799</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="16">
         <v>39.366939410484797</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="17">
         <v>10.5604001735816</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
         <v>1.3552924823078401</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="16">
         <v>39.364514617192199</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="17">
         <v>10.565811118848799</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="12">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
         <v>1.3222490411299901</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="19">
         <v>39.362578959500802</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="20">
         <v>10.572195251627599</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
         <v>1.4733913525596301</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="16">
         <v>26.970137383669599</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="17">
         <v>10.5824093581729</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
         <v>1.3568759703675499</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="16">
         <v>26.9636125083324</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="17">
         <v>10.5956241732629</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
         <v>1.4018463858055199</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="16">
         <v>26.958989030978501</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="17">
         <v>10.6043105571427</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
         <v>1.3865631146245601</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="16">
         <v>26.955886375619698</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="17">
         <v>10.610120536077</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="12">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
         <v>1.4040378911585301</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="19">
         <v>26.953250865529199</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="20">
         <v>10.618763672176099</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="8">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="15">
         <v>1.90442677260824</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="16">
         <v>8.8059358933331193</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="17">
         <v>10.650167987968</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
         <v>1.9246256233936601</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="16">
         <v>8.8021926995501207</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="17">
         <v>10.6695323485059</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="8">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="15">
         <v>1.97316691579315</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="16">
         <v>8.7999387951474901</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="17">
         <v>10.6890922209835</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="8">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
         <v>2.0371468588497899</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="16">
         <v>8.7960833383889394</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="17">
         <v>10.704030775544</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="12">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
         <v>1.95802685433298</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="19">
         <v>8.7919021362321104</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="20">
         <v>10.718738989345701</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>